<commit_message>
Update FORMATO ENVIO REPORTES MAS SERVICIOS.xlsx
</commit_message>
<xml_diff>
--- a/MAS SERVICIOS RELACION/FORMATO ENVIO REPORTES MAS SERVICIOS.xlsx
+++ b/MAS SERVICIOS RELACION/FORMATO ENVIO REPORTES MAS SERVICIOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GRUAS NUÑEZ SA DE CV\Desktop\MAS SERVICIOS RELACION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GRUAS NUÑEZ SA DE CV\Desktop\REPOSITORIO-GRUAS-2019\MAS SERVICIOS RELACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4FFE4D-4A73-4AB5-96F9-A39D1C4ACC7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7899E791-DF7B-4F6A-85F2-AD035F53FC4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORMATO DE CAPTURA" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
   <si>
     <t>LOCAL/FORANEO</t>
   </si>
@@ -213,6 +214,66 @@
   </si>
   <si>
     <t>ENERO</t>
+  </si>
+  <si>
+    <t>MS1920180</t>
+  </si>
+  <si>
+    <t>NISSAN NP300</t>
+  </si>
+  <si>
+    <t>TETECALA MOR</t>
+  </si>
+  <si>
+    <t>LAZARO CARDENAS, CUERNAVACA MOR</t>
+  </si>
+  <si>
+    <t>JUNIO</t>
+  </si>
+  <si>
+    <t>MS1920907</t>
+  </si>
+  <si>
+    <t>CAMBION DE LLANTA</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>AUDI A5</t>
+  </si>
+  <si>
+    <t>CLUB NAUTICO TEQUESQUITENGO MOR</t>
+  </si>
+  <si>
+    <t>MISMO</t>
+  </si>
+  <si>
+    <t>MS1922096</t>
+  </si>
+  <si>
+    <t>GM CHEVY</t>
+  </si>
+  <si>
+    <t>AUT MEX-ACA KM 128</t>
+  </si>
+  <si>
+    <t>IZTACALCO CDMX</t>
+  </si>
+  <si>
+    <t>MS1949889</t>
+  </si>
+  <si>
+    <t>VW JETTA</t>
+  </si>
+  <si>
+    <t>AUT MEX-ACA KM 119</t>
+  </si>
+  <si>
+    <t>CENTRO, CUERNAVACA MOR</t>
+  </si>
+  <si>
+    <t>FEBRERO</t>
   </si>
 </sst>
 </file>
@@ -296,7 +357,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +379,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -456,6 +523,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -480,20 +562,8 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -563,7 +633,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="28574" y="57149"/>
-          <a:ext cx="2276475" cy="868481"/>
+          <a:ext cx="2329815" cy="866576"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -996,10 +1066,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:XFC142"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1037,17 +1110,17 @@
     <row r="2" spans="1:21 16378:16380" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:21 16378:16380" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:21 16378:16380" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="37" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="8" t="s">
         <v>26</v>
       </c>
@@ -1057,11 +1130,11 @@
       <c r="J4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="39" t="s">
+      <c r="K4" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="XEX4" s="10" t="s">
@@ -1075,27 +1148,27 @@
       </c>
     </row>
     <row r="5" spans="1:21 16378:16380" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="37" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="36">
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="41">
         <v>43494</v>
       </c>
-      <c r="I5" s="36"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="40">
+      <c r="I5" s="41"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="45">
         <v>0.5</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="XEX5" s="10" t="s">
@@ -1109,23 +1182,23 @@
       </c>
     </row>
     <row r="6" spans="1:21 16378:16380" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="37" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="XEX6" s="10" t="s">
@@ -1212,14 +1285,14 @@
         <v>885.84</v>
       </c>
     </row>
-    <row r="8" spans="1:21 16378:16380" s="45" customFormat="1" ht="48" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:21 16378:16380" s="37" customFormat="1" ht="48" x14ac:dyDescent="0.3">
+      <c r="A8" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="34" t="s">
         <v>50</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -1231,20 +1304,20 @@
       <c r="F8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42" t="s">
+      <c r="J8" s="34"/>
+      <c r="K8" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="L8" s="44">
+      <c r="L8" s="36">
         <v>2200</v>
       </c>
       <c r="M8" s="18">
@@ -1259,19 +1332,15 @@
         <f>L8+M8-N8</f>
         <v>2464</v>
       </c>
-      <c r="P8" s="15">
-        <v>62</v>
-      </c>
-      <c r="Q8" s="15">
-        <v>108</v>
-      </c>
-      <c r="R8" s="44">
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="36">
         <v>0</v>
       </c>
-      <c r="S8" s="44">
+      <c r="S8" s="36">
         <v>0</v>
       </c>
-      <c r="T8" s="44">
+      <c r="T8" s="36">
         <f>P8*R8+S8</f>
         <v>0</v>
       </c>
@@ -1313,7 +1382,7 @@
         <v>3900</v>
       </c>
       <c r="M9" s="18">
-        <f t="shared" ref="M9" si="0">L9*0.16</f>
+        <f t="shared" ref="M9:M10" si="0">L9*0.16</f>
         <v>624</v>
       </c>
       <c r="N9" s="18">
@@ -1324,9 +1393,7 @@
         <f>L9+M9-N9</f>
         <v>4368</v>
       </c>
-      <c r="P9" s="15">
-        <v>10</v>
-      </c>
+      <c r="P9" s="15"/>
       <c r="Q9" s="14"/>
       <c r="R9" s="14">
         <v>0</v>
@@ -1334,28 +1401,59 @@
       <c r="S9" s="14">
         <v>0</v>
       </c>
-      <c r="T9" s="44">
+      <c r="T9" s="36">
         <f>P9*R9+S9</f>
         <v>0</v>
       </c>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21 16378:16380" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+    <row r="10" spans="1:21 16378:16380" s="16" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>63</v>
+      </c>
       <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
+      <c r="K10" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="17">
+        <v>3903.45</v>
+      </c>
+      <c r="M10" s="18">
+        <f t="shared" si="0"/>
+        <v>624.55200000000002</v>
+      </c>
+      <c r="N10" s="18">
+        <f>L10*0.04</f>
+        <v>156.13800000000001</v>
+      </c>
+      <c r="O10" s="18">
+        <f>L10+M10-N10</f>
+        <v>4371.8639999999996</v>
+      </c>
       <c r="P10" s="15"/>
       <c r="Q10" s="14"/>
       <c r="R10" s="14"/>
@@ -1363,22 +1461,52 @@
       <c r="T10" s="14"/>
       <c r="U10" s="31"/>
     </row>
-    <row r="11" spans="1:21 16378:16380" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+    <row r="11" spans="1:21 16378:16380" s="16" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>70</v>
+      </c>
       <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
+      <c r="K11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="14">
+        <v>2100</v>
+      </c>
+      <c r="M11" s="18">
+        <f t="shared" ref="M11:M13" si="1">L11*0.16</f>
+        <v>336</v>
+      </c>
+      <c r="N11" s="18">
+        <v>0</v>
+      </c>
+      <c r="O11" s="18">
+        <f>L11+M11-N11</f>
+        <v>2436</v>
+      </c>
       <c r="P11" s="15"/>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
@@ -1387,21 +1515,52 @@
       <c r="U11" s="31"/>
     </row>
     <row r="12" spans="1:21 16378:16380" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="A12" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
+      <c r="K12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="14">
+        <v>7500</v>
+      </c>
+      <c r="M12" s="18">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="N12" s="18">
+        <f>L12*0.04</f>
+        <v>300</v>
+      </c>
+      <c r="O12" s="18">
+        <f>L12+M12-N12</f>
+        <v>8400</v>
+      </c>
       <c r="P12" s="15"/>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
@@ -1409,22 +1568,53 @@
       <c r="T12" s="14"/>
       <c r="U12" s="31"/>
     </row>
-    <row r="13" spans="1:21 16378:16380" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
+    <row r="13" spans="1:21 16378:16380" s="16" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
+      <c r="K13" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="14">
+        <v>3015.52</v>
+      </c>
+      <c r="M13" s="18">
+        <f t="shared" si="1"/>
+        <v>482.48320000000001</v>
+      </c>
+      <c r="N13" s="18">
+        <f>L13*0.04</f>
+        <v>120.6208</v>
+      </c>
+      <c r="O13" s="18">
+        <f>L13+M13-N13</f>
+        <v>3377.3824</v>
+      </c>
       <c r="P13" s="15"/>
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
@@ -1446,8 +1636,13 @@
       <c r="K14" s="11"/>
       <c r="L14" s="14"/>
       <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
+      <c r="N14" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="O14" s="46">
+        <f>SUM(O8:O13)</f>
+        <v>25417.2464</v>
+      </c>
       <c r="P14" s="15"/>
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
@@ -2077,35 +2272,35 @@
       <c r="U41" s="31"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J42" s="33" t="s">
+      <c r="J42" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="K42" s="34"/>
+      <c r="K42" s="39"/>
       <c r="L42" s="17">
         <f>SUM(L8:L41)</f>
-        <v>6100</v>
+        <v>22618.97</v>
       </c>
       <c r="M42" s="30">
         <f>SUM(M8:M41)</f>
-        <v>976</v>
+        <v>3619.0352000000003</v>
       </c>
       <c r="N42" s="30">
         <f>SUM(N8:N41)</f>
-        <v>244</v>
+        <v>820.75880000000006</v>
       </c>
       <c r="O42" s="30">
         <f>SUM(O8:O41)</f>
-        <v>6832</v>
+        <v>50834.4928</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J43" s="33" t="s">
+      <c r="J43" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="K43" s="34"/>
+      <c r="K43" s="39"/>
       <c r="L43" s="17">
         <f>L42*16%</f>
-        <v>976</v>
+        <v>3619.0352000000003</v>
       </c>
       <c r="M43" s="19"/>
     </row>
@@ -2116,29 +2311,29 @@
       <c r="K44" s="24"/>
       <c r="L44" s="17">
         <f>L42+L43</f>
-        <v>7076</v>
+        <v>26238.0052</v>
       </c>
       <c r="M44" s="19"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J45" s="33" t="s">
+      <c r="J45" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="K45" s="34"/>
+      <c r="K45" s="39"/>
       <c r="L45" s="14">
         <f>SUM(N8:N41)</f>
-        <v>244</v>
+        <v>820.75880000000006</v>
       </c>
       <c r="M45" s="20"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J46" s="33" t="s">
+      <c r="J46" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="K46" s="34"/>
+      <c r="K46" s="39"/>
       <c r="L46" s="21">
         <f>L42+L43-L45</f>
-        <v>6832</v>
+        <v>25417.2464</v>
       </c>
       <c r="M46" s="22"/>
     </row>
@@ -2277,7 +2472,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="26" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="45" orientation="landscape" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="20" min="3" max="67" man="1"/>
   </colBreaks>

</xml_diff>